<commit_message>
carol's final timesheet for week 4
</commit_message>
<xml_diff>
--- a/admin/Timesheets/Caroline Chang/Week 4 Timesheet.xlsx
+++ b/admin/Timesheets/Caroline Chang/Week 4 Timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carol\CSCI_Classes\CSCI4308\capstone_proj\admin\Timesheets\Caroline Chang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DE1736A-540A-40BD-A04E-8D31FCB7BCEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EBC9C3F-9539-4679-B160-A654FB0A031F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2652" yWindow="1956" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,9 +42,6 @@
     <t>Read/Study</t>
   </si>
   <si>
-    <t>Sponsor Meeting</t>
-  </si>
-  <si>
     <t>Team Meeting</t>
   </si>
   <si>
@@ -64,6 +61,9 @@
   </si>
   <si>
     <t>Work Emails</t>
+  </si>
+  <si>
+    <t>Testing Old Code</t>
   </si>
 </sst>
 </file>
@@ -421,7 +421,7 @@
   <dimension ref="A4:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -437,7 +437,7 @@
         <v>0</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -466,13 +466,13 @@
         <v>44843</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>1</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -494,7 +494,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D8">
         <v>0.5</v>
@@ -505,13 +505,18 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="I9" s="1"/>
+        <v>12</v>
+      </c>
+      <c r="G9">
+        <v>0.5</v>
+      </c>
+      <c r="I9" s="1">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10">
         <v>0.5</v>
@@ -522,7 +527,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11">
         <v>0.5</v>
@@ -533,7 +538,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B12" s="1">
         <v>2.5</v>
@@ -544,10 +549,12 @@
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
+      <c r="G12" s="1">
+        <v>0.5</v>
+      </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1">
-        <v>3</v>
+        <v>3.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>